<commit_message>
Finished up Assignment 3
</commit_message>
<xml_diff>
--- a/SVC Results.xlsx
+++ b/SVC Results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\najia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/602b5d9235103c93/Desktop/AUS/CMP-466 Machine Learning/Project/ML-Rainfall-Forecasting-Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE7F202-BBD6-4980-B761-4D0E47A4939A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="80" documentId="13_ncr:1_{BBE7F202-BBD6-4980-B761-4D0E47A4939A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FA620349-B2FC-40AC-BD97-DAD6591DA386}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4390" yWindow="2280" windowWidth="17330" windowHeight="15350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Classifier</t>
   </si>
@@ -69,9 +69,6 @@
     <t>gamma=auto, C=default</t>
   </si>
   <si>
-    <t>degree..</t>
-  </si>
-  <si>
     <t>avg training acc</t>
   </si>
   <si>
@@ -106,6 +103,12 @@
   </si>
   <si>
     <t>degree = 10</t>
+  </si>
+  <si>
+    <t>As we can see In the above table, the highest overall accuracy we got was for SVC 'Linear Kernel' and the worst accuracy we got was from the 'Sigmoid Kernel'. For RBF, the best values if gamma we found was the default one which used the 1 / (n_features * X.var()) as value of gamma. We found out that lower the value of gamma better the accuracy was. For c, the best accuracy was for 10 after which the accuracy didnt improve by much and started to lower again</t>
+  </si>
+  <si>
+    <t>degree = default (3)</t>
   </si>
 </sst>
 </file>
@@ -218,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -226,6 +229,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -234,9 +244,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -247,10 +254,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -531,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:P18"/>
+  <dimension ref="B3:P23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -565,25 +572,25 @@
       <c r="D3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="7"/>
-      <c r="J3" s="12" t="s">
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="8" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="2:16" x14ac:dyDescent="0.35">
@@ -609,7 +616,7 @@
       <c r="I4" s="4">
         <v>0.76178959999999996</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <f>AVERAGE(E4:I4)</f>
         <v>0.74634856799999993</v>
       </c>
@@ -628,7 +635,7 @@
       <c r="O4" s="2">
         <v>0.7038835</v>
       </c>
-      <c r="P4" s="2">
+      <c r="P4" s="1">
         <f>AVERAGE(K4:O4)</f>
         <v>0.69423573199999988</v>
       </c>
@@ -658,7 +665,7 @@
       <c r="I5" s="2">
         <v>0.83555018000000003</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <f t="shared" ref="J5:J15" si="0">AVERAGE(E5:I5)</f>
         <v>0.84656815400000007</v>
       </c>
@@ -677,7 +684,7 @@
       <c r="O5" s="2">
         <v>0.86407767000000002</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <f t="shared" ref="P5:P15" si="1">AVERAGE(K5:O5)</f>
         <v>0.78324656399999992</v>
       </c>
@@ -691,29 +698,29 @@
         <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>0.77966102000000004</v>
+        <v>1</v>
       </c>
       <c r="F6" s="2">
-        <v>0.74334140000000004</v>
+        <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>0.54600484000000005</v>
+        <v>1</v>
       </c>
       <c r="H6" s="2">
-        <v>0.56348246999999996</v>
+        <v>1</v>
       </c>
       <c r="I6" s="2">
-        <v>0.54655381000000003</v>
-      </c>
-      <c r="J6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="1">
         <f t="shared" si="0"/>
-        <v>0.63580870800000011</v>
-      </c>
-      <c r="K6" s="3">
-        <v>0.69565217000000001</v>
-      </c>
-      <c r="L6" s="3">
-        <v>0.72946860000000002</v>
+        <v>1</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.50241546000000004</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.57971013999999998</v>
       </c>
       <c r="M6" s="3">
         <v>0.50724638</v>
@@ -724,9 +731,9 @@
       <c r="O6" s="3">
         <v>0.51456310999999999</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <f t="shared" si="1"/>
-        <v>0.60006566399999994</v>
+        <v>0.53146662999999994</v>
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.35">
@@ -735,7 +742,7 @@
         <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2">
         <v>1</v>
@@ -752,7 +759,7 @@
       <c r="I7" s="2">
         <v>1</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -771,7 +778,7 @@
       <c r="O7" s="2">
         <v>0.5</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <f t="shared" si="1"/>
         <v>0.50531400999999998</v>
       </c>
@@ -782,7 +789,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="2">
         <v>0.77966102000000004</v>
@@ -799,7 +806,7 @@
       <c r="I8" s="2">
         <v>0.54655381000000003</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="1">
         <f t="shared" si="0"/>
         <v>0.63580870800000011</v>
       </c>
@@ -818,7 +825,7 @@
       <c r="O8" s="2">
         <v>0.51456310999999999</v>
       </c>
-      <c r="P8" s="2">
+      <c r="P8" s="1">
         <f t="shared" si="1"/>
         <v>0.60006566399999994</v>
       </c>
@@ -827,7 +834,7 @@
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E9" s="2">
         <v>0.79782081999999999</v>
@@ -844,7 +851,7 @@
       <c r="I9" s="2">
         <v>0.77146311999999995</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <f t="shared" si="0"/>
         <v>0.783403356</v>
       </c>
@@ -863,7 +870,7 @@
       <c r="O9" s="2">
         <v>0.80582524</v>
       </c>
-      <c r="P9" s="2">
+      <c r="P9" s="1">
         <f t="shared" si="1"/>
         <v>0.77737911199999998</v>
       </c>
@@ -872,7 +879,7 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10" s="2">
         <v>0.82808716999999998</v>
@@ -889,7 +896,7 @@
       <c r="I10" s="2">
         <v>0.79443772999999995</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <f t="shared" si="0"/>
         <v>0.81172036000000003</v>
       </c>
@@ -908,7 +915,7 @@
       <c r="O10" s="2">
         <v>0.83495145999999998</v>
       </c>
-      <c r="P10" s="2">
+      <c r="P10" s="1">
         <f t="shared" si="1"/>
         <v>0.78517424199999997</v>
       </c>
@@ -917,7 +924,7 @@
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="2">
         <v>0.82808716999999998</v>
@@ -934,7 +941,7 @@
       <c r="I11" s="2">
         <v>0.79443772999999995</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <f t="shared" si="0"/>
         <v>0.81172036000000003</v>
       </c>
@@ -953,7 +960,7 @@
       <c r="O11" s="2">
         <v>0.83495145999999998</v>
       </c>
-      <c r="P11" s="2">
+      <c r="P11" s="1">
         <f t="shared" si="1"/>
         <v>0.78517424199999997</v>
       </c>
@@ -979,7 +986,7 @@
       <c r="I12" s="2">
         <v>0.50060459000000002</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <f t="shared" si="0"/>
         <v>0.59055660399999998</v>
       </c>
@@ -998,7 +1005,7 @@
       <c r="O12" s="2">
         <v>0.5</v>
       </c>
-      <c r="P12" s="2">
+      <c r="P12" s="1">
         <f t="shared" si="1"/>
         <v>0.56425120600000001</v>
       </c>
@@ -1009,7 +1016,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E13" s="2">
         <v>0.78571429000000004</v>
@@ -1026,7 +1033,7 @@
       <c r="I13" s="2">
         <v>0.75695283999999996</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <f t="shared" si="0"/>
         <v>0.76573366999999992</v>
       </c>
@@ -1045,7 +1052,7 @@
       <c r="O13" s="2">
         <v>0.79126213999999995</v>
       </c>
-      <c r="P13" s="2">
+      <c r="P13" s="1">
         <f t="shared" si="1"/>
         <v>0.762844144</v>
       </c>
@@ -1054,7 +1061,7 @@
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E14" s="2">
         <v>0.79418886</v>
@@ -1071,7 +1078,7 @@
       <c r="I14" s="2">
         <v>0.76783555000000003</v>
       </c>
-      <c r="J14" s="2">
+      <c r="J14" s="1">
         <f t="shared" si="0"/>
         <v>0.77953101999999996</v>
       </c>
@@ -1090,7 +1097,7 @@
       <c r="O14" s="2">
         <v>0.81553397999999999</v>
       </c>
-      <c r="P14" s="2">
+      <c r="P14" s="1">
         <f t="shared" si="1"/>
         <v>0.77157732000000001</v>
       </c>
@@ -1099,7 +1106,7 @@
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15" s="2">
         <v>0.81113800999999996</v>
@@ -1116,7 +1123,7 @@
       <c r="I15" s="2">
         <v>0.78718259000000002</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="1">
         <f t="shared" si="0"/>
         <v>0.79695711599999997</v>
       </c>
@@ -1135,24 +1142,78 @@
       <c r="O15" s="2">
         <v>0.82038834999999999</v>
       </c>
-      <c r="P15" s="2">
+      <c r="P15" s="1">
         <f t="shared" si="1"/>
         <v>0.78029642199999993</v>
       </c>
     </row>
     <row r="16" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="J16" s="13"/>
-      <c r="P16" s="13"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="J16" s="7"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="J17" s="14">
+        <f>MIN(J4:J15)</f>
+        <v>0.59055660399999998</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>14</v>
-      </c>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B19" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="15"/>
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="15"/>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="K3:O3"/>
+    <mergeCell ref="B19:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>